<commit_message>
made sure tests functioned sequentially and added other features
</commit_message>
<xml_diff>
--- a/RegData.xlsx
+++ b/RegData.xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0" showInkAnnotation="0"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="17820" windowWidth="25040" xWindow="9020" yWindow="1680"/>
+    <workbookView xWindow="320" yWindow="3600" windowWidth="8000" windowHeight="17820" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>RegNum</t>
   </si>
@@ -33,10 +33,55 @@
     <t>WHITE</t>
   </si>
   <si>
-    <t>PN11 MOU</t>
-  </si>
-  <si>
-    <t>MK60 VUL</t>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>EF63 YPZ</t>
+  </si>
+  <si>
+    <t>KY66 LNU</t>
+  </si>
+  <si>
+    <t>PE65 YNY</t>
+  </si>
+  <si>
+    <t>FORD</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>SMART</t>
+  </si>
+  <si>
+    <t>BLACK</t>
+  </si>
+  <si>
+    <t>RENAULT</t>
+  </si>
+  <si>
+    <t>YC11 OMK</t>
+  </si>
+  <si>
+    <t>UK65 FCV</t>
+  </si>
+  <si>
+    <t>KR66 NUO</t>
+  </si>
+  <si>
+    <t>MINI</t>
+  </si>
+  <si>
+    <t>SILVER</t>
+  </si>
+  <si>
+    <t>TOYOTA</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>SUZUKI</t>
   </si>
   <si>
     <t>Pass</t>
@@ -46,11 +91,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -73,17 +133,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -92,10 +160,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -249,7 +317,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -258,13 +326,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -274,7 +342,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -283,7 +351,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -292,7 +360,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -302,12 +370,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -338,7 +406,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -357,7 +425,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -408,47 +476,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
converted to cucumber after cucumber revision
</commit_message>
<xml_diff>
--- a/RegData.xlsx
+++ b/RegData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Java EE Project\RegPlates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="320" yWindow="3600" windowWidth="8000" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="315" yWindow="3600" windowWidth="7995" windowHeight="17820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -152,6 +157,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -480,12 +493,12 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -513,7 +526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -527,7 +540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -541,7 +554,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -555,7 +568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -569,7 +582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
ensured fail cases, added exceptions and also chrome driver
</commit_message>
<xml_diff>
--- a/RegData.xlsx
+++ b/RegData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
   <si>
     <t>RegNum</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -591,10 +594,10 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>